<commit_message>
Reading data from excel file.
</commit_message>
<xml_diff>
--- a/YourCart_Automation/src/main/java/com/Yourcart/qa/TestData/YourcartTestData.xlsx
+++ b/YourCart_Automation/src/main/java/com/Yourcart/qa/TestData/YourcartTestData.xlsx
@@ -3,19 +3,15 @@
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
   <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="24332"/>
   <workbookPr defaultThemeVersion="166925"/>
-  <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
-    <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\prita\Downloads\"/>
-    </mc:Choice>
-  </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="8_{3819BD07-E045-4BBD-A5C7-741C16B2A18E}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:801_{452040A9-3E1D-421F-9D62-D6708AE15612}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-108" yWindow="-108" windowWidth="23256" windowHeight="13176" xr2:uid="{A6E12A25-0CFA-4014-B583-30E668D8B44A}"/>
   </bookViews>
   <sheets>
-    <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
+    <sheet name="Login" sheetId="1" r:id="rId1"/>
   </sheets>
-  <calcPr calcId="191029"/>
+  <calcPr calcId="0"/>
+  <oleSize ref="A1"/>
   <extLst>
     <ext xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" uri="{140A7094-0E35-4892-8432-C4D2E57EDEB5}">
       <x15:workbookPr chartTrackingRefBase="1"/>
@@ -24,9 +20,38 @@
 </workbook>
 </file>
 
+<file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="8" uniqueCount="8">
+  <si>
+    <t>Email</t>
+  </si>
+  <si>
+    <t>Password</t>
+  </si>
+  <si>
+    <t>ketif98663@ikowat.com</t>
+  </si>
+  <si>
+    <t>ketif98663</t>
+  </si>
+  <si>
+    <t>ketif9866@ikowat.com</t>
+  </si>
+  <si>
+    <t>ketif983@ikowat.com</t>
+  </si>
+  <si>
+    <t>ketif98664</t>
+  </si>
+  <si>
+    <t>ketif98665</t>
+  </si>
+</sst>
+</file>
+
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="x14ac x16r2 xr">
-  <fonts count="1" x14ac:knownFonts="1">
+  <fonts count="3" x14ac:knownFonts="1">
     <font>
       <sz val="11"/>
       <color theme="1"/>
@@ -34,16 +59,36 @@
       <family val="2"/>
       <scheme val="minor"/>
     </font>
+    <font>
+      <u/>
+      <sz val="11"/>
+      <color theme="10"/>
+      <name val="Calibri"/>
+      <family val="2"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <sz val="8"/>
+      <name val="Calibri"/>
+      <family val="2"/>
+      <scheme val="minor"/>
+    </font>
   </fonts>
-  <fills count="2">
+  <fills count="3">
     <fill>
       <patternFill patternType="none"/>
     </fill>
     <fill>
       <patternFill patternType="gray125"/>
     </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor rgb="FFFFFF00"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
   </fills>
-  <borders count="1">
+  <borders count="2">
     <border>
       <left/>
       <right/>
@@ -51,14 +96,36 @@
       <bottom/>
       <diagonal/>
     </border>
+    <border>
+      <left style="thin">
+        <color indexed="64"/>
+      </left>
+      <right style="thin">
+        <color indexed="64"/>
+      </right>
+      <top style="thin">
+        <color indexed="64"/>
+      </top>
+      <bottom style="thin">
+        <color indexed="64"/>
+      </bottom>
+      <diagonal/>
+    </border>
   </borders>
-  <cellStyleXfs count="1">
+  <cellStyleXfs count="2">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
   </cellStyleXfs>
-  <cellXfs count="1">
+  <cellXfs count="6">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
+    <xf numFmtId="49" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
+    <xf numFmtId="49" fontId="0" fillId="2" borderId="1" xfId="0" applyNumberFormat="1" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="0" fillId="2" borderId="1" xfId="0" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="49" fontId="1" fillId="0" borderId="1" xfId="1" applyNumberFormat="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" applyBorder="1"/>
   </cellXfs>
-  <cellStyles count="1">
+  <cellStyles count="2">
+    <cellStyle name="Hyperlink" xfId="1" builtinId="8"/>
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
   </cellStyles>
   <dxfs count="0"/>
@@ -371,12 +438,57 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{EF131D64-34B9-4E9B-A242-66314B18C0EB}">
-  <dimension ref="A1"/>
+  <dimension ref="A1:B4"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0"/>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
-  <sheetData/>
+  <cols>
+    <col min="1" max="1" width="21.44140625" style="1" bestFit="1" customWidth="1"/>
+    <col min="2" max="2" width="9.6640625" bestFit="1" customWidth="1"/>
+  </cols>
+  <sheetData>
+    <row r="1" spans="1:2" x14ac:dyDescent="0.3">
+      <c r="A1" s="2" t="s">
+        <v>0</v>
+      </c>
+      <c r="B1" s="3" t="s">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="2" spans="1:2" x14ac:dyDescent="0.3">
+      <c r="A2" s="4" t="s">
+        <v>2</v>
+      </c>
+      <c r="B2" s="5" t="s">
+        <v>3</v>
+      </c>
+    </row>
+    <row r="3" spans="1:2" x14ac:dyDescent="0.3">
+      <c r="A3" s="4" t="s">
+        <v>4</v>
+      </c>
+      <c r="B3" s="5" t="s">
+        <v>6</v>
+      </c>
+    </row>
+    <row r="4" spans="1:2" x14ac:dyDescent="0.3">
+      <c r="A4" s="4" t="s">
+        <v>5</v>
+      </c>
+      <c r="B4" s="5" t="s">
+        <v>7</v>
+      </c>
+    </row>
+  </sheetData>
+  <phoneticPr fontId="2" type="noConversion"/>
+  <hyperlinks>
+    <hyperlink ref="A2" r:id="rId1" xr:uid="{16A51402-9453-4C4C-ABAE-CAF4CAE59FDA}"/>
+    <hyperlink ref="A3:A4" r:id="rId2" display="ketif98663@ikowat.com" xr:uid="{E6AFC9AD-6AFC-4C7F-BDAB-59F77B0AA905}"/>
+    <hyperlink ref="A3" r:id="rId3" xr:uid="{D97BDA0A-EF11-4C37-933C-733DB942034A}"/>
+    <hyperlink ref="A4" r:id="rId4" xr:uid="{FDB18364-97FE-4F8C-816F-ADC7EA861012}"/>
+  </hyperlinks>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+  <pageSetup orientation="portrait" r:id="rId5"/>
 </worksheet>
 </file>
</xml_diff>